<commit_message>
update data mining homework
</commit_message>
<xml_diff>
--- a/October Assignment Calendar.xlsx
+++ b/October Assignment Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\MSA\GitHub\bluefall2hwteam17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{1D443825-AF63-4E7B-BA42-BEC76A681631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DC2A151-73B4-4385-8802-E66258D11DCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,14 +304,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="7" applyFont="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -640,7 +640,7 @@
   <dimension ref="B1:H15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,10 +657,10 @@
         <f ca="1">YEAR(TODAY())</f>
         <v>2022</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="10"/>
+      <c r="D1" s="11"/>
       <c r="E1" s="8" t="s">
         <v>0</v>
       </c>
@@ -669,10 +669,10 @@
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="11"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
@@ -777,17 +777,17 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="G7" s="5" t="s">
         <v>11</v>
       </c>
@@ -915,11 +915,11 @@
       <c r="B13" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="6"/>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F13" s="5" t="s">

</xml_diff>